<commit_message>
added more photo to gallery & fixed ancor issue
</commit_message>
<xml_diff>
--- a/menu_files/gallery.xlsx
+++ b/menu_files/gallery.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="314">
   <si>
     <t>&lt;a href="img/gallery-page/</t>
   </si>
@@ -578,6 +578,390 @@
   </si>
   <si>
     <t>.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/</t>
+  </si>
+  <si>
+    <t>Honey__0001</t>
+  </si>
+  <si>
+    <t>Honey__0002</t>
+  </si>
+  <si>
+    <t>Honey__0003</t>
+  </si>
+  <si>
+    <t>Honey__0004</t>
+  </si>
+  <si>
+    <t>Honey__0005</t>
+  </si>
+  <si>
+    <t>Honey__0006</t>
+  </si>
+  <si>
+    <t>Honey__0007</t>
+  </si>
+  <si>
+    <t>Honey__0008</t>
+  </si>
+  <si>
+    <t>Honey__0009</t>
+  </si>
+  <si>
+    <t>Honey__0010</t>
+  </si>
+  <si>
+    <t>Honey__0011</t>
+  </si>
+  <si>
+    <t>Honey__0012</t>
+  </si>
+  <si>
+    <t>Honey__0013</t>
+  </si>
+  <si>
+    <t>Honey__0014</t>
+  </si>
+  <si>
+    <t>Honey__0015</t>
+  </si>
+  <si>
+    <t>Honey__0016</t>
+  </si>
+  <si>
+    <t>Honey__0017</t>
+  </si>
+  <si>
+    <t>Honey__0018</t>
+  </si>
+  <si>
+    <t>Honey__0019</t>
+  </si>
+  <si>
+    <t>Honey__0020</t>
+  </si>
+  <si>
+    <t>Honey__0021</t>
+  </si>
+  <si>
+    <t>Honey__0022</t>
+  </si>
+  <si>
+    <t>Honey__0023</t>
+  </si>
+  <si>
+    <t>Honey__0024</t>
+  </si>
+  <si>
+    <t>Honey__0025</t>
+  </si>
+  <si>
+    <t>Honey__0026</t>
+  </si>
+  <si>
+    <t>Honey__0027</t>
+  </si>
+  <si>
+    <t>Honey__0028</t>
+  </si>
+  <si>
+    <t>Honey__0029</t>
+  </si>
+  <si>
+    <t>Honey__0030</t>
+  </si>
+  <si>
+    <t>Honey__0031</t>
+  </si>
+  <si>
+    <t>Honey__0032</t>
+  </si>
+  <si>
+    <t>Honey__0033</t>
+  </si>
+  <si>
+    <t>Honey__0034</t>
+  </si>
+  <si>
+    <t>Honey__0035</t>
+  </si>
+  <si>
+    <t>Honey__0036</t>
+  </si>
+  <si>
+    <t>Honey__0037</t>
+  </si>
+  <si>
+    <t>Honey__0038</t>
+  </si>
+  <si>
+    <t>Honey__0039</t>
+  </si>
+  <si>
+    <t>Honey__0040</t>
+  </si>
+  <si>
+    <t>Honey__0041</t>
+  </si>
+  <si>
+    <t>Honey__0042</t>
+  </si>
+  <si>
+    <t>Honey__0043</t>
+  </si>
+  <si>
+    <t>Honey__0044</t>
+  </si>
+  <si>
+    <t>Honey__0045</t>
+  </si>
+  <si>
+    <t>Honey__0046</t>
+  </si>
+  <si>
+    <t>Honey__0047</t>
+  </si>
+  <si>
+    <t>Honey__0048</t>
+  </si>
+  <si>
+    <t>Honey__0049</t>
+  </si>
+  <si>
+    <t>Honey__0050</t>
+  </si>
+  <si>
+    <t>Honey__0051</t>
+  </si>
+  <si>
+    <t>Honey__0052</t>
+  </si>
+  <si>
+    <t>Honey__0053</t>
+  </si>
+  <si>
+    <t>Honey__0054</t>
+  </si>
+  <si>
+    <t>Honey__0055</t>
+  </si>
+  <si>
+    <t>Honey__0056</t>
+  </si>
+  <si>
+    <t>Honey__0057</t>
+  </si>
+  <si>
+    <t>Honey__0058</t>
+  </si>
+  <si>
+    <t>Honey__0059</t>
+  </si>
+  <si>
+    <t>Honey__0060</t>
+  </si>
+  <si>
+    <t>Honey__0061</t>
+  </si>
+  <si>
+    <t>Honey__0062</t>
+  </si>
+  <si>
+    <t>Honey__0063</t>
+  </si>
+  <si>
+    <t>Honey__0064</t>
+  </si>
+  <si>
+    <t>119 214</t>
+  </si>
+  <si>
+    <t>127 392</t>
+  </si>
+  <si>
+    <t>129 992</t>
+  </si>
+  <si>
+    <t>140 021</t>
+  </si>
+  <si>
+    <t>133 837</t>
+  </si>
+  <si>
+    <t>115 257</t>
+  </si>
+  <si>
+    <t>111 172</t>
+  </si>
+  <si>
+    <t>146 427</t>
+  </si>
+  <si>
+    <t>127 302</t>
+  </si>
+  <si>
+    <t>119 066</t>
+  </si>
+  <si>
+    <t>141 962</t>
+  </si>
+  <si>
+    <t>135 805</t>
+  </si>
+  <si>
+    <t>168 675</t>
+  </si>
+  <si>
+    <t>172 488</t>
+  </si>
+  <si>
+    <t>194 582</t>
+  </si>
+  <si>
+    <t>161 680</t>
+  </si>
+  <si>
+    <t>140 752</t>
+  </si>
+  <si>
+    <t>138 805</t>
+  </si>
+  <si>
+    <t>192 762</t>
+  </si>
+  <si>
+    <t>131 383</t>
+  </si>
+  <si>
+    <t>153 848</t>
+  </si>
+  <si>
+    <t>176 489</t>
+  </si>
+  <si>
+    <t>227 562</t>
+  </si>
+  <si>
+    <t>170 976</t>
+  </si>
+  <si>
+    <t>195 767</t>
+  </si>
+  <si>
+    <t>157 000</t>
+  </si>
+  <si>
+    <t>160 922</t>
+  </si>
+  <si>
+    <t>117 168</t>
+  </si>
+  <si>
+    <t>139 188</t>
+  </si>
+  <si>
+    <t>144 161</t>
+  </si>
+  <si>
+    <t>168 619</t>
+  </si>
+  <si>
+    <t>161 401</t>
+  </si>
+  <si>
+    <t>172 852</t>
+  </si>
+  <si>
+    <t>205 970</t>
+  </si>
+  <si>
+    <t>157 674</t>
+  </si>
+  <si>
+    <t>148 321</t>
+  </si>
+  <si>
+    <t>130 878</t>
+  </si>
+  <si>
+    <t>126 128</t>
+  </si>
+  <si>
+    <t>151 449</t>
+  </si>
+  <si>
+    <t>158 495</t>
+  </si>
+  <si>
+    <t>153 604</t>
+  </si>
+  <si>
+    <t>169 676</t>
+  </si>
+  <si>
+    <t>168 134</t>
+  </si>
+  <si>
+    <t>162 889</t>
+  </si>
+  <si>
+    <t>171 974</t>
+  </si>
+  <si>
+    <t>154 693</t>
+  </si>
+  <si>
+    <t>127 345</t>
+  </si>
+  <si>
+    <t>130 370</t>
+  </si>
+  <si>
+    <t>136 484</t>
+  </si>
+  <si>
+    <t>156 258</t>
+  </si>
+  <si>
+    <t>134 008</t>
+  </si>
+  <si>
+    <t>175 118</t>
+  </si>
+  <si>
+    <t>203 311</t>
+  </si>
+  <si>
+    <t>140 465</t>
+  </si>
+  <si>
+    <t>196 620</t>
+  </si>
+  <si>
+    <t>148 813</t>
+  </si>
+  <si>
+    <t>154 335</t>
+  </si>
+  <si>
+    <t>176 910</t>
+  </si>
+  <si>
+    <t>177 975</t>
+  </si>
+  <si>
+    <t>180 466</t>
+  </si>
+  <si>
+    <t>203 809</t>
+  </si>
+  <si>
+    <t>173 076</t>
+  </si>
+  <si>
+    <t>166 254</t>
+  </si>
+  <si>
+    <t>148 433</t>
   </si>
 </sst>
 </file>
@@ -922,16 +1306,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J114"/>
+  <dimension ref="A1:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="J109" sqref="J109:J114"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="J116" sqref="J116:J179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.8" customHeight="1">
@@ -4709,6 +5096,2183 @@
         <f t="shared" si="5"/>
         <v>&lt;a href="img/gallery-page/guests/big/IMG_7969.jpg" class="block-gallery__image"&gt;
        &lt;picture&gt;&lt;source srcset="img/gallery-page/guests/small/IMG_7969.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/IMG_7969.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" s="4" customFormat="1"/>
+    <row r="116" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A116" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s">
+        <v>186</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F116" t="s">
+        <v>186</v>
+      </c>
+      <c r="G116" t="s">
+        <v>185</v>
+      </c>
+      <c r="H116" t="s">
+        <v>186</v>
+      </c>
+      <c r="I116" t="s">
+        <v>54</v>
+      </c>
+      <c r="J116" t="str">
+        <f t="shared" ref="J116" si="6">CONCATENATE(A116,B116,C116,D116,E116,F116,G116,H116,I116)</f>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0001.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0001.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0001.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A117" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>187</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F117" t="s">
+        <v>187</v>
+      </c>
+      <c r="G117" t="s">
+        <v>185</v>
+      </c>
+      <c r="H117" t="s">
+        <v>187</v>
+      </c>
+      <c r="I117" t="s">
+        <v>54</v>
+      </c>
+      <c r="J117" t="str">
+        <f t="shared" ref="J117:J179" si="7">CONCATENATE(A117,B117,C117,D117,E117,F117,G117,H117,I117)</f>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0002.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0002.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0002.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118" t="s">
+        <v>188</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F118" t="s">
+        <v>188</v>
+      </c>
+      <c r="G118" t="s">
+        <v>185</v>
+      </c>
+      <c r="H118" t="s">
+        <v>188</v>
+      </c>
+      <c r="I118" t="s">
+        <v>54</v>
+      </c>
+      <c r="J118" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0003.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0003.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0003.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A119" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2</v>
+      </c>
+      <c r="D119" t="s">
+        <v>189</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F119" t="s">
+        <v>189</v>
+      </c>
+      <c r="G119" t="s">
+        <v>185</v>
+      </c>
+      <c r="H119" t="s">
+        <v>189</v>
+      </c>
+      <c r="I119" t="s">
+        <v>54</v>
+      </c>
+      <c r="J119" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0004.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0004.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0004.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s">
+        <v>190</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F120" t="s">
+        <v>190</v>
+      </c>
+      <c r="G120" t="s">
+        <v>185</v>
+      </c>
+      <c r="H120" t="s">
+        <v>190</v>
+      </c>
+      <c r="I120" t="s">
+        <v>54</v>
+      </c>
+      <c r="J120" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0005.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0005.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0005.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121" t="s">
+        <v>191</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F121" t="s">
+        <v>191</v>
+      </c>
+      <c r="G121" t="s">
+        <v>185</v>
+      </c>
+      <c r="H121" t="s">
+        <v>191</v>
+      </c>
+      <c r="I121" t="s">
+        <v>54</v>
+      </c>
+      <c r="J121" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0006.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0006.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0006.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A122" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122" t="s">
+        <v>192</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F122" t="s">
+        <v>192</v>
+      </c>
+      <c r="G122" t="s">
+        <v>185</v>
+      </c>
+      <c r="H122" t="s">
+        <v>192</v>
+      </c>
+      <c r="I122" t="s">
+        <v>54</v>
+      </c>
+      <c r="J122" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0007.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0007.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0007.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A123" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>2</v>
+      </c>
+      <c r="D123" t="s">
+        <v>193</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F123" t="s">
+        <v>193</v>
+      </c>
+      <c r="G123" t="s">
+        <v>185</v>
+      </c>
+      <c r="H123" t="s">
+        <v>193</v>
+      </c>
+      <c r="I123" t="s">
+        <v>54</v>
+      </c>
+      <c r="J123" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0008.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0008.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0008.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A124" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+      <c r="D124" t="s">
+        <v>194</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F124" t="s">
+        <v>194</v>
+      </c>
+      <c r="G124" t="s">
+        <v>185</v>
+      </c>
+      <c r="H124" t="s">
+        <v>194</v>
+      </c>
+      <c r="I124" t="s">
+        <v>54</v>
+      </c>
+      <c r="J124" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0009.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0009.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0009.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A125" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+      <c r="D125" t="s">
+        <v>195</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F125" t="s">
+        <v>195</v>
+      </c>
+      <c r="G125" t="s">
+        <v>185</v>
+      </c>
+      <c r="H125" t="s">
+        <v>195</v>
+      </c>
+      <c r="I125" t="s">
+        <v>54</v>
+      </c>
+      <c r="J125" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0010.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0010.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0010.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>2</v>
+      </c>
+      <c r="D126" t="s">
+        <v>196</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F126" t="s">
+        <v>196</v>
+      </c>
+      <c r="G126" t="s">
+        <v>185</v>
+      </c>
+      <c r="H126" t="s">
+        <v>196</v>
+      </c>
+      <c r="I126" t="s">
+        <v>54</v>
+      </c>
+      <c r="J126" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0011.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0011.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0011.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A127" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>2</v>
+      </c>
+      <c r="D127" t="s">
+        <v>197</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F127" t="s">
+        <v>197</v>
+      </c>
+      <c r="G127" t="s">
+        <v>185</v>
+      </c>
+      <c r="H127" t="s">
+        <v>197</v>
+      </c>
+      <c r="I127" t="s">
+        <v>54</v>
+      </c>
+      <c r="J127" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0012.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0012.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0012.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A128" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2</v>
+      </c>
+      <c r="D128" t="s">
+        <v>198</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F128" t="s">
+        <v>198</v>
+      </c>
+      <c r="G128" t="s">
+        <v>185</v>
+      </c>
+      <c r="H128" t="s">
+        <v>198</v>
+      </c>
+      <c r="I128" t="s">
+        <v>54</v>
+      </c>
+      <c r="J128" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0013.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0013.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0013.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A129" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>2</v>
+      </c>
+      <c r="D129" t="s">
+        <v>199</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F129" t="s">
+        <v>199</v>
+      </c>
+      <c r="G129" t="s">
+        <v>185</v>
+      </c>
+      <c r="H129" t="s">
+        <v>199</v>
+      </c>
+      <c r="I129" t="s">
+        <v>54</v>
+      </c>
+      <c r="J129" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0014.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0014.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0014.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A130" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>2</v>
+      </c>
+      <c r="D130" t="s">
+        <v>200</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F130" t="s">
+        <v>200</v>
+      </c>
+      <c r="G130" t="s">
+        <v>185</v>
+      </c>
+      <c r="H130" t="s">
+        <v>200</v>
+      </c>
+      <c r="I130" t="s">
+        <v>54</v>
+      </c>
+      <c r="J130" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0015.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0015.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0015.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A131" t="s">
+        <v>0</v>
+      </c>
+      <c r="B131" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" t="s">
+        <v>2</v>
+      </c>
+      <c r="D131" t="s">
+        <v>201</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F131" t="s">
+        <v>201</v>
+      </c>
+      <c r="G131" t="s">
+        <v>185</v>
+      </c>
+      <c r="H131" t="s">
+        <v>201</v>
+      </c>
+      <c r="I131" t="s">
+        <v>54</v>
+      </c>
+      <c r="J131" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0016.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0016.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0016.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A132" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" t="s">
+        <v>1</v>
+      </c>
+      <c r="C132" t="s">
+        <v>2</v>
+      </c>
+      <c r="D132" t="s">
+        <v>202</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F132" t="s">
+        <v>202</v>
+      </c>
+      <c r="G132" t="s">
+        <v>185</v>
+      </c>
+      <c r="H132" t="s">
+        <v>202</v>
+      </c>
+      <c r="I132" t="s">
+        <v>54</v>
+      </c>
+      <c r="J132" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0017.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0017.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0017.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A133" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2</v>
+      </c>
+      <c r="D133" t="s">
+        <v>203</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F133" t="s">
+        <v>203</v>
+      </c>
+      <c r="G133" t="s">
+        <v>185</v>
+      </c>
+      <c r="H133" t="s">
+        <v>203</v>
+      </c>
+      <c r="I133" t="s">
+        <v>54</v>
+      </c>
+      <c r="J133" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0018.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0018.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0018.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A134" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>2</v>
+      </c>
+      <c r="D134" t="s">
+        <v>204</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F134" t="s">
+        <v>204</v>
+      </c>
+      <c r="G134" t="s">
+        <v>185</v>
+      </c>
+      <c r="H134" t="s">
+        <v>204</v>
+      </c>
+      <c r="I134" t="s">
+        <v>54</v>
+      </c>
+      <c r="J134" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0019.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0019.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0019.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A135" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" t="s">
+        <v>2</v>
+      </c>
+      <c r="D135" t="s">
+        <v>205</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F135" t="s">
+        <v>205</v>
+      </c>
+      <c r="G135" t="s">
+        <v>185</v>
+      </c>
+      <c r="H135" t="s">
+        <v>205</v>
+      </c>
+      <c r="I135" t="s">
+        <v>54</v>
+      </c>
+      <c r="J135" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0020.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0020.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0020.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A136" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>2</v>
+      </c>
+      <c r="D136" t="s">
+        <v>206</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F136" t="s">
+        <v>206</v>
+      </c>
+      <c r="G136" t="s">
+        <v>185</v>
+      </c>
+      <c r="H136" t="s">
+        <v>206</v>
+      </c>
+      <c r="I136" t="s">
+        <v>54</v>
+      </c>
+      <c r="J136" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0021.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0021.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0021.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D137" t="s">
+        <v>207</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F137" t="s">
+        <v>207</v>
+      </c>
+      <c r="G137" t="s">
+        <v>185</v>
+      </c>
+      <c r="H137" t="s">
+        <v>207</v>
+      </c>
+      <c r="I137" t="s">
+        <v>54</v>
+      </c>
+      <c r="J137" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0022.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0022.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0022.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A138" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" t="s">
+        <v>2</v>
+      </c>
+      <c r="D138" t="s">
+        <v>208</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F138" t="s">
+        <v>208</v>
+      </c>
+      <c r="G138" t="s">
+        <v>185</v>
+      </c>
+      <c r="H138" t="s">
+        <v>208</v>
+      </c>
+      <c r="I138" t="s">
+        <v>54</v>
+      </c>
+      <c r="J138" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0023.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0023.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0023.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A139" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139" t="s">
+        <v>209</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F139" t="s">
+        <v>209</v>
+      </c>
+      <c r="G139" t="s">
+        <v>185</v>
+      </c>
+      <c r="H139" t="s">
+        <v>209</v>
+      </c>
+      <c r="I139" t="s">
+        <v>54</v>
+      </c>
+      <c r="J139" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0024.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0024.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0024.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2</v>
+      </c>
+      <c r="D140" t="s">
+        <v>210</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F140" t="s">
+        <v>210</v>
+      </c>
+      <c r="G140" t="s">
+        <v>185</v>
+      </c>
+      <c r="H140" t="s">
+        <v>210</v>
+      </c>
+      <c r="I140" t="s">
+        <v>54</v>
+      </c>
+      <c r="J140" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0025.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0025.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0025.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A141" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+      <c r="D141" t="s">
+        <v>211</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F141" t="s">
+        <v>211</v>
+      </c>
+      <c r="G141" t="s">
+        <v>185</v>
+      </c>
+      <c r="H141" t="s">
+        <v>211</v>
+      </c>
+      <c r="I141" t="s">
+        <v>54</v>
+      </c>
+      <c r="J141" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0026.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0026.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0026.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A142" t="s">
+        <v>0</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
+        <v>2</v>
+      </c>
+      <c r="D142" t="s">
+        <v>212</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F142" t="s">
+        <v>212</v>
+      </c>
+      <c r="G142" t="s">
+        <v>185</v>
+      </c>
+      <c r="H142" t="s">
+        <v>212</v>
+      </c>
+      <c r="I142" t="s">
+        <v>54</v>
+      </c>
+      <c r="J142" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0027.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0027.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0027.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A143" t="s">
+        <v>0</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
+        <v>2</v>
+      </c>
+      <c r="D143" t="s">
+        <v>213</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F143" t="s">
+        <v>213</v>
+      </c>
+      <c r="G143" t="s">
+        <v>185</v>
+      </c>
+      <c r="H143" t="s">
+        <v>213</v>
+      </c>
+      <c r="I143" t="s">
+        <v>54</v>
+      </c>
+      <c r="J143" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0028.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0028.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0028.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A144" t="s">
+        <v>0</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
+        <v>2</v>
+      </c>
+      <c r="D144" t="s">
+        <v>214</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F144" t="s">
+        <v>214</v>
+      </c>
+      <c r="G144" t="s">
+        <v>185</v>
+      </c>
+      <c r="H144" t="s">
+        <v>214</v>
+      </c>
+      <c r="I144" t="s">
+        <v>54</v>
+      </c>
+      <c r="J144" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0029.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0029.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0029.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A145" t="s">
+        <v>0</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1</v>
+      </c>
+      <c r="C145" t="s">
+        <v>2</v>
+      </c>
+      <c r="D145" t="s">
+        <v>215</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F145" t="s">
+        <v>215</v>
+      </c>
+      <c r="G145" t="s">
+        <v>185</v>
+      </c>
+      <c r="H145" t="s">
+        <v>215</v>
+      </c>
+      <c r="I145" t="s">
+        <v>54</v>
+      </c>
+      <c r="J145" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0030.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0030.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0030.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A146" t="s">
+        <v>0</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s">
+        <v>2</v>
+      </c>
+      <c r="D146" t="s">
+        <v>216</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F146" t="s">
+        <v>216</v>
+      </c>
+      <c r="G146" t="s">
+        <v>185</v>
+      </c>
+      <c r="H146" t="s">
+        <v>216</v>
+      </c>
+      <c r="I146" t="s">
+        <v>54</v>
+      </c>
+      <c r="J146" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0031.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0031.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0031.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A147" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2</v>
+      </c>
+      <c r="D147" t="s">
+        <v>217</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F147" t="s">
+        <v>217</v>
+      </c>
+      <c r="G147" t="s">
+        <v>185</v>
+      </c>
+      <c r="H147" t="s">
+        <v>217</v>
+      </c>
+      <c r="I147" t="s">
+        <v>54</v>
+      </c>
+      <c r="J147" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0032.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0032.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0032.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A148" t="s">
+        <v>0</v>
+      </c>
+      <c r="B148" t="s">
+        <v>1</v>
+      </c>
+      <c r="C148" t="s">
+        <v>2</v>
+      </c>
+      <c r="D148" t="s">
+        <v>218</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F148" t="s">
+        <v>218</v>
+      </c>
+      <c r="G148" t="s">
+        <v>185</v>
+      </c>
+      <c r="H148" t="s">
+        <v>218</v>
+      </c>
+      <c r="I148" t="s">
+        <v>54</v>
+      </c>
+      <c r="J148" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0033.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0033.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0033.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A149" t="s">
+        <v>0</v>
+      </c>
+      <c r="B149" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" t="s">
+        <v>2</v>
+      </c>
+      <c r="D149" t="s">
+        <v>219</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F149" t="s">
+        <v>219</v>
+      </c>
+      <c r="G149" t="s">
+        <v>185</v>
+      </c>
+      <c r="H149" t="s">
+        <v>219</v>
+      </c>
+      <c r="I149" t="s">
+        <v>54</v>
+      </c>
+      <c r="J149" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0034.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0034.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0034.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A150" t="s">
+        <v>0</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" t="s">
+        <v>2</v>
+      </c>
+      <c r="D150" t="s">
+        <v>220</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F150" t="s">
+        <v>220</v>
+      </c>
+      <c r="G150" t="s">
+        <v>185</v>
+      </c>
+      <c r="H150" t="s">
+        <v>220</v>
+      </c>
+      <c r="I150" t="s">
+        <v>54</v>
+      </c>
+      <c r="J150" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0035.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0035.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0035.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A151" t="s">
+        <v>0</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2</v>
+      </c>
+      <c r="D151" t="s">
+        <v>221</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F151" t="s">
+        <v>221</v>
+      </c>
+      <c r="G151" t="s">
+        <v>185</v>
+      </c>
+      <c r="H151" t="s">
+        <v>221</v>
+      </c>
+      <c r="I151" t="s">
+        <v>54</v>
+      </c>
+      <c r="J151" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0036.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0036.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0036.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A152" t="s">
+        <v>0</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>2</v>
+      </c>
+      <c r="D152" t="s">
+        <v>222</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F152" t="s">
+        <v>222</v>
+      </c>
+      <c r="G152" t="s">
+        <v>185</v>
+      </c>
+      <c r="H152" t="s">
+        <v>222</v>
+      </c>
+      <c r="I152" t="s">
+        <v>54</v>
+      </c>
+      <c r="J152" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0037.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0037.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0037.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A153" t="s">
+        <v>0</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" t="s">
+        <v>2</v>
+      </c>
+      <c r="D153" t="s">
+        <v>223</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F153" t="s">
+        <v>223</v>
+      </c>
+      <c r="G153" t="s">
+        <v>185</v>
+      </c>
+      <c r="H153" t="s">
+        <v>223</v>
+      </c>
+      <c r="I153" t="s">
+        <v>54</v>
+      </c>
+      <c r="J153" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0038.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0038.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0038.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A154" t="s">
+        <v>0</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154" t="s">
+        <v>2</v>
+      </c>
+      <c r="D154" t="s">
+        <v>224</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F154" t="s">
+        <v>224</v>
+      </c>
+      <c r="G154" t="s">
+        <v>185</v>
+      </c>
+      <c r="H154" t="s">
+        <v>224</v>
+      </c>
+      <c r="I154" t="s">
+        <v>54</v>
+      </c>
+      <c r="J154" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0039.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0039.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0039.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A155" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>2</v>
+      </c>
+      <c r="D155" t="s">
+        <v>225</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F155" t="s">
+        <v>225</v>
+      </c>
+      <c r="G155" t="s">
+        <v>185</v>
+      </c>
+      <c r="H155" t="s">
+        <v>225</v>
+      </c>
+      <c r="I155" t="s">
+        <v>54</v>
+      </c>
+      <c r="J155" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0040.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0040.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0040.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A156" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1</v>
+      </c>
+      <c r="C156" t="s">
+        <v>2</v>
+      </c>
+      <c r="D156" t="s">
+        <v>226</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F156" t="s">
+        <v>226</v>
+      </c>
+      <c r="G156" t="s">
+        <v>185</v>
+      </c>
+      <c r="H156" t="s">
+        <v>226</v>
+      </c>
+      <c r="I156" t="s">
+        <v>54</v>
+      </c>
+      <c r="J156" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0041.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0041.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0041.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A157" t="s">
+        <v>0</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157" t="s">
+        <v>2</v>
+      </c>
+      <c r="D157" t="s">
+        <v>227</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F157" t="s">
+        <v>227</v>
+      </c>
+      <c r="G157" t="s">
+        <v>185</v>
+      </c>
+      <c r="H157" t="s">
+        <v>227</v>
+      </c>
+      <c r="I157" t="s">
+        <v>54</v>
+      </c>
+      <c r="J157" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0042.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0042.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0042.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A158" t="s">
+        <v>0</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158" t="s">
+        <v>2</v>
+      </c>
+      <c r="D158" t="s">
+        <v>228</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F158" t="s">
+        <v>228</v>
+      </c>
+      <c r="G158" t="s">
+        <v>185</v>
+      </c>
+      <c r="H158" t="s">
+        <v>228</v>
+      </c>
+      <c r="I158" t="s">
+        <v>54</v>
+      </c>
+      <c r="J158" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0043.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0043.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0043.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A159" t="s">
+        <v>0</v>
+      </c>
+      <c r="B159" t="s">
+        <v>1</v>
+      </c>
+      <c r="C159" t="s">
+        <v>2</v>
+      </c>
+      <c r="D159" t="s">
+        <v>229</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F159" t="s">
+        <v>229</v>
+      </c>
+      <c r="G159" t="s">
+        <v>185</v>
+      </c>
+      <c r="H159" t="s">
+        <v>229</v>
+      </c>
+      <c r="I159" t="s">
+        <v>54</v>
+      </c>
+      <c r="J159" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0044.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0044.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0044.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2</v>
+      </c>
+      <c r="D160" t="s">
+        <v>230</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F160" t="s">
+        <v>230</v>
+      </c>
+      <c r="G160" t="s">
+        <v>185</v>
+      </c>
+      <c r="H160" t="s">
+        <v>230</v>
+      </c>
+      <c r="I160" t="s">
+        <v>54</v>
+      </c>
+      <c r="J160" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0045.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0045.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0045.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A161" t="s">
+        <v>0</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161" t="s">
+        <v>2</v>
+      </c>
+      <c r="D161" t="s">
+        <v>231</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F161" t="s">
+        <v>231</v>
+      </c>
+      <c r="G161" t="s">
+        <v>185</v>
+      </c>
+      <c r="H161" t="s">
+        <v>231</v>
+      </c>
+      <c r="I161" t="s">
+        <v>54</v>
+      </c>
+      <c r="J161" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0046.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0046.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0046.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A162" t="s">
+        <v>0</v>
+      </c>
+      <c r="B162" t="s">
+        <v>1</v>
+      </c>
+      <c r="C162" t="s">
+        <v>2</v>
+      </c>
+      <c r="D162" t="s">
+        <v>232</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F162" t="s">
+        <v>232</v>
+      </c>
+      <c r="G162" t="s">
+        <v>185</v>
+      </c>
+      <c r="H162" t="s">
+        <v>232</v>
+      </c>
+      <c r="I162" t="s">
+        <v>54</v>
+      </c>
+      <c r="J162" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0047.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0047.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0047.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A163" t="s">
+        <v>0</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" t="s">
+        <v>2</v>
+      </c>
+      <c r="D163" t="s">
+        <v>233</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F163" t="s">
+        <v>233</v>
+      </c>
+      <c r="G163" t="s">
+        <v>185</v>
+      </c>
+      <c r="H163" t="s">
+        <v>233</v>
+      </c>
+      <c r="I163" t="s">
+        <v>54</v>
+      </c>
+      <c r="J163" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0048.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0048.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0048.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A164" t="s">
+        <v>0</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164" t="s">
+        <v>2</v>
+      </c>
+      <c r="D164" t="s">
+        <v>234</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F164" t="s">
+        <v>234</v>
+      </c>
+      <c r="G164" t="s">
+        <v>185</v>
+      </c>
+      <c r="H164" t="s">
+        <v>234</v>
+      </c>
+      <c r="I164" t="s">
+        <v>54</v>
+      </c>
+      <c r="J164" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0049.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0049.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0049.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A165" t="s">
+        <v>0</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" t="s">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>235</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F165" t="s">
+        <v>235</v>
+      </c>
+      <c r="G165" t="s">
+        <v>185</v>
+      </c>
+      <c r="H165" t="s">
+        <v>235</v>
+      </c>
+      <c r="I165" t="s">
+        <v>54</v>
+      </c>
+      <c r="J165" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0050.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0050.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0050.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166" t="s">
+        <v>2</v>
+      </c>
+      <c r="D166" t="s">
+        <v>236</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F166" t="s">
+        <v>236</v>
+      </c>
+      <c r="G166" t="s">
+        <v>185</v>
+      </c>
+      <c r="H166" t="s">
+        <v>236</v>
+      </c>
+      <c r="I166" t="s">
+        <v>54</v>
+      </c>
+      <c r="J166" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0051.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0051.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0051.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A167" t="s">
+        <v>0</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1</v>
+      </c>
+      <c r="C167" t="s">
+        <v>2</v>
+      </c>
+      <c r="D167" t="s">
+        <v>237</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F167" t="s">
+        <v>237</v>
+      </c>
+      <c r="G167" t="s">
+        <v>185</v>
+      </c>
+      <c r="H167" t="s">
+        <v>237</v>
+      </c>
+      <c r="I167" t="s">
+        <v>54</v>
+      </c>
+      <c r="J167" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0052.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0052.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0052.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A168" t="s">
+        <v>0</v>
+      </c>
+      <c r="B168" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
+        <v>2</v>
+      </c>
+      <c r="D168" t="s">
+        <v>238</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F168" t="s">
+        <v>238</v>
+      </c>
+      <c r="G168" t="s">
+        <v>185</v>
+      </c>
+      <c r="H168" t="s">
+        <v>238</v>
+      </c>
+      <c r="I168" t="s">
+        <v>54</v>
+      </c>
+      <c r="J168" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0053.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0053.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0053.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A169" t="s">
+        <v>0</v>
+      </c>
+      <c r="B169" t="s">
+        <v>1</v>
+      </c>
+      <c r="C169" t="s">
+        <v>2</v>
+      </c>
+      <c r="D169" t="s">
+        <v>239</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F169" t="s">
+        <v>239</v>
+      </c>
+      <c r="G169" t="s">
+        <v>185</v>
+      </c>
+      <c r="H169" t="s">
+        <v>239</v>
+      </c>
+      <c r="I169" t="s">
+        <v>54</v>
+      </c>
+      <c r="J169" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0054.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0054.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0054.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A170" t="s">
+        <v>0</v>
+      </c>
+      <c r="B170" t="s">
+        <v>1</v>
+      </c>
+      <c r="C170" t="s">
+        <v>2</v>
+      </c>
+      <c r="D170" t="s">
+        <v>240</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F170" t="s">
+        <v>240</v>
+      </c>
+      <c r="G170" t="s">
+        <v>185</v>
+      </c>
+      <c r="H170" t="s">
+        <v>240</v>
+      </c>
+      <c r="I170" t="s">
+        <v>54</v>
+      </c>
+      <c r="J170" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0055.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0055.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0055.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A171" t="s">
+        <v>0</v>
+      </c>
+      <c r="B171" t="s">
+        <v>1</v>
+      </c>
+      <c r="C171" t="s">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>241</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F171" t="s">
+        <v>241</v>
+      </c>
+      <c r="G171" t="s">
+        <v>185</v>
+      </c>
+      <c r="H171" t="s">
+        <v>241</v>
+      </c>
+      <c r="I171" t="s">
+        <v>54</v>
+      </c>
+      <c r="J171" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0056.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0056.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0056.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A172" t="s">
+        <v>0</v>
+      </c>
+      <c r="B172" t="s">
+        <v>1</v>
+      </c>
+      <c r="C172" t="s">
+        <v>2</v>
+      </c>
+      <c r="D172" t="s">
+        <v>242</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F172" t="s">
+        <v>242</v>
+      </c>
+      <c r="G172" t="s">
+        <v>185</v>
+      </c>
+      <c r="H172" t="s">
+        <v>242</v>
+      </c>
+      <c r="I172" t="s">
+        <v>54</v>
+      </c>
+      <c r="J172" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0057.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0057.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0057.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A173" t="s">
+        <v>0</v>
+      </c>
+      <c r="B173" t="s">
+        <v>1</v>
+      </c>
+      <c r="C173" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>243</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F173" t="s">
+        <v>243</v>
+      </c>
+      <c r="G173" t="s">
+        <v>185</v>
+      </c>
+      <c r="H173" t="s">
+        <v>243</v>
+      </c>
+      <c r="I173" t="s">
+        <v>54</v>
+      </c>
+      <c r="J173" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0058.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0058.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0058.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A174" t="s">
+        <v>0</v>
+      </c>
+      <c r="B174" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174" t="s">
+        <v>2</v>
+      </c>
+      <c r="D174" t="s">
+        <v>244</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F174" t="s">
+        <v>244</v>
+      </c>
+      <c r="G174" t="s">
+        <v>185</v>
+      </c>
+      <c r="H174" t="s">
+        <v>244</v>
+      </c>
+      <c r="I174" t="s">
+        <v>54</v>
+      </c>
+      <c r="J174" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0059.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0059.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0059.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A175" t="s">
+        <v>0</v>
+      </c>
+      <c r="B175" t="s">
+        <v>1</v>
+      </c>
+      <c r="C175" t="s">
+        <v>2</v>
+      </c>
+      <c r="D175" t="s">
+        <v>245</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F175" t="s">
+        <v>245</v>
+      </c>
+      <c r="G175" t="s">
+        <v>185</v>
+      </c>
+      <c r="H175" t="s">
+        <v>245</v>
+      </c>
+      <c r="I175" t="s">
+        <v>54</v>
+      </c>
+      <c r="J175" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0060.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0060.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0060.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A176" t="s">
+        <v>0</v>
+      </c>
+      <c r="B176" t="s">
+        <v>1</v>
+      </c>
+      <c r="C176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D176" t="s">
+        <v>246</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F176" t="s">
+        <v>246</v>
+      </c>
+      <c r="G176" t="s">
+        <v>185</v>
+      </c>
+      <c r="H176" t="s">
+        <v>246</v>
+      </c>
+      <c r="I176" t="s">
+        <v>54</v>
+      </c>
+      <c r="J176" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0061.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0061.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0061.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A177" t="s">
+        <v>0</v>
+      </c>
+      <c r="B177" t="s">
+        <v>1</v>
+      </c>
+      <c r="C177" t="s">
+        <v>2</v>
+      </c>
+      <c r="D177" t="s">
+        <v>247</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F177" t="s">
+        <v>247</v>
+      </c>
+      <c r="G177" t="s">
+        <v>185</v>
+      </c>
+      <c r="H177" t="s">
+        <v>247</v>
+      </c>
+      <c r="I177" t="s">
+        <v>54</v>
+      </c>
+      <c r="J177" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0062.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0062.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0062.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178" t="s">
+        <v>2</v>
+      </c>
+      <c r="D178" t="s">
+        <v>248</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F178" t="s">
+        <v>248</v>
+      </c>
+      <c r="G178" t="s">
+        <v>185</v>
+      </c>
+      <c r="H178" t="s">
+        <v>248</v>
+      </c>
+      <c r="I178" t="s">
+        <v>54</v>
+      </c>
+      <c r="J178" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0063.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0063.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0063.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" ht="13.2" customHeight="1">
+      <c r="A179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B179" t="s">
+        <v>1</v>
+      </c>
+      <c r="C179" t="s">
+        <v>2</v>
+      </c>
+      <c r="D179" t="s">
+        <v>249</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F179" t="s">
+        <v>249</v>
+      </c>
+      <c r="G179" t="s">
+        <v>185</v>
+      </c>
+      <c r="H179" t="s">
+        <v>249</v>
+      </c>
+      <c r="I179" t="s">
+        <v>54</v>
+      </c>
+      <c r="J179" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;a href="img/gallery-page/cuisin/big/Honey__0064.jpg" class="block-gallery__image"&gt;
+       &lt;picture&gt;&lt;source srcset="img/gallery-page/cuisin/small/Honey__0064.webp" type="image/webp"&gt;&lt;img src="img/gallery-page/guests/small/Honey__0064.jpg" alt="image dish"&gt;&lt;/picture&gt;&lt;/a&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -4718,10 +7282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58:D63"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65:D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5564,6 +8128,902 @@
       </c>
       <c r="D63" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B65" s="3">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="C65" t="s">
+        <v>250</v>
+      </c>
+      <c r="D65" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B66" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C66" t="s">
+        <v>251</v>
+      </c>
+      <c r="D66" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B67" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C67" t="s">
+        <v>252</v>
+      </c>
+      <c r="D67" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B68" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C68" t="s">
+        <v>253</v>
+      </c>
+      <c r="D68" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B69" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C69" t="s">
+        <v>254</v>
+      </c>
+      <c r="D69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B70" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C70" t="s">
+        <v>255</v>
+      </c>
+      <c r="D70" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B71" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C71" t="s">
+        <v>256</v>
+      </c>
+      <c r="D71" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B72" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C72" t="s">
+        <v>257</v>
+      </c>
+      <c r="D72" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C73" t="s">
+        <v>258</v>
+      </c>
+      <c r="D73" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B74" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C74" t="s">
+        <v>259</v>
+      </c>
+      <c r="D74" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B75" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C75" t="s">
+        <v>260</v>
+      </c>
+      <c r="D75" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B76" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C76" t="s">
+        <v>261</v>
+      </c>
+      <c r="D76" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B77" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C77" t="s">
+        <v>262</v>
+      </c>
+      <c r="D77" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B78" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C78" t="s">
+        <v>263</v>
+      </c>
+      <c r="D78" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B79" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C79" t="s">
+        <v>264</v>
+      </c>
+      <c r="D79" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B80" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C80" t="s">
+        <v>265</v>
+      </c>
+      <c r="D80" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B81" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C81" t="s">
+        <v>266</v>
+      </c>
+      <c r="D81" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B82" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C82" t="s">
+        <v>267</v>
+      </c>
+      <c r="D82" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B83" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D83" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B84" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C84" t="s">
+        <v>269</v>
+      </c>
+      <c r="D84" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B85" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C85" t="s">
+        <v>270</v>
+      </c>
+      <c r="D85" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B86" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C86" t="s">
+        <v>271</v>
+      </c>
+      <c r="D86" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B87" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C87" t="s">
+        <v>272</v>
+      </c>
+      <c r="D87" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B88" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C88" t="s">
+        <v>273</v>
+      </c>
+      <c r="D88" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B89" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C89" t="s">
+        <v>274</v>
+      </c>
+      <c r="D89" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B90" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C90" t="s">
+        <v>275</v>
+      </c>
+      <c r="D90" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B91" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C91" t="s">
+        <v>276</v>
+      </c>
+      <c r="D91" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B92" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C92" t="s">
+        <v>277</v>
+      </c>
+      <c r="D92" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B93" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C93" t="s">
+        <v>278</v>
+      </c>
+      <c r="D93" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B94" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C94" t="s">
+        <v>279</v>
+      </c>
+      <c r="D94" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B95" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C95" t="s">
+        <v>280</v>
+      </c>
+      <c r="D95" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B96" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C96" t="s">
+        <v>281</v>
+      </c>
+      <c r="D96" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B97" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C97" t="s">
+        <v>282</v>
+      </c>
+      <c r="D97" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B98" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C98" t="s">
+        <v>283</v>
+      </c>
+      <c r="D98" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B99" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C99" t="s">
+        <v>284</v>
+      </c>
+      <c r="D99" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B100" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C100" t="s">
+        <v>285</v>
+      </c>
+      <c r="D100" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B101" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C101" t="s">
+        <v>286</v>
+      </c>
+      <c r="D101" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B102" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C102" t="s">
+        <v>287</v>
+      </c>
+      <c r="D102" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B103" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C103" t="s">
+        <v>288</v>
+      </c>
+      <c r="D103" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B104" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C104" t="s">
+        <v>289</v>
+      </c>
+      <c r="D104" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B105" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C105" t="s">
+        <v>290</v>
+      </c>
+      <c r="D105" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B106" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C106" t="s">
+        <v>291</v>
+      </c>
+      <c r="D106" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B107" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C107" t="s">
+        <v>292</v>
+      </c>
+      <c r="D107" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B108" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C108" t="s">
+        <v>293</v>
+      </c>
+      <c r="D108" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B109" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C109" t="s">
+        <v>294</v>
+      </c>
+      <c r="D109" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B110" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C110" t="s">
+        <v>295</v>
+      </c>
+      <c r="D110" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B111" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C111" t="s">
+        <v>296</v>
+      </c>
+      <c r="D111" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B112" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C112" t="s">
+        <v>297</v>
+      </c>
+      <c r="D112" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B113" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C113" t="s">
+        <v>298</v>
+      </c>
+      <c r="D113" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B114" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C114" t="s">
+        <v>299</v>
+      </c>
+      <c r="D114" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B115" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C115" t="s">
+        <v>300</v>
+      </c>
+      <c r="D115" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B116" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C116" t="s">
+        <v>301</v>
+      </c>
+      <c r="D116" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B117" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C117" t="s">
+        <v>302</v>
+      </c>
+      <c r="D117" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B118" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C118" t="s">
+        <v>303</v>
+      </c>
+      <c r="D118" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B119" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C119" t="s">
+        <v>304</v>
+      </c>
+      <c r="D119" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B120" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C120" t="s">
+        <v>305</v>
+      </c>
+      <c r="D120" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B121" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C121" t="s">
+        <v>306</v>
+      </c>
+      <c r="D121" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B122" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C122" t="s">
+        <v>307</v>
+      </c>
+      <c r="D122" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B123" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C123" t="s">
+        <v>308</v>
+      </c>
+      <c r="D123" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B124" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C124" t="s">
+        <v>309</v>
+      </c>
+      <c r="D124" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B125" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C125" t="s">
+        <v>310</v>
+      </c>
+      <c r="D125" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B126" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C126" t="s">
+        <v>311</v>
+      </c>
+      <c r="D126" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B127" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C127" t="s">
+        <v>312</v>
+      </c>
+      <c r="D127" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B128" s="3">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="C128" t="s">
+        <v>313</v>
+      </c>
+      <c r="D128" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>